<commit_message>
Skip sending emails for entries without an email address
</commit_message>
<xml_diff>
--- a/anantya.xlsx
+++ b/anantya.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4309" uniqueCount="1976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4340" uniqueCount="1983">
   <si>
     <t xml:space="preserve">Student Name </t>
   </si>
@@ -5449,9 +5449,15 @@
     <t>Nimisha Pandey</t>
   </si>
   <si>
+    <t>nimisha.pandey24@pccoepune.org</t>
+  </si>
+  <si>
     <t>Ishita B Deb</t>
   </si>
   <si>
+    <t>PIYUSH.AHIRAO23@PCCOEPUNE.ORG</t>
+  </si>
+  <si>
     <t>sumitrachaure914@gmail.com</t>
   </si>
   <si>
@@ -5467,9 +5473,15 @@
     <t>Ashish Patil</t>
   </si>
   <si>
+    <t>ashish.patil23@pccoepune.org</t>
+  </si>
+  <si>
     <t>Prajwal Hage</t>
   </si>
   <si>
+    <t>prajwal.hage23@pccoepune.org</t>
+  </si>
+  <si>
     <t>Samiksha Mote</t>
   </si>
   <si>
@@ -5509,6 +5521,9 @@
     <t>Kushagra Gupta</t>
   </si>
   <si>
+    <t>kushagra.gupta23@pccoepune.org</t>
+  </si>
+  <si>
     <t>Himanshu Patil</t>
   </si>
   <si>
@@ -5524,9 +5539,15 @@
     <t>Aaryan Nerkar</t>
   </si>
   <si>
+    <t>aaryan.nerkar24@pccoepune.org</t>
+  </si>
+  <si>
     <t>Rushikesh Mahavir Kurundwade</t>
   </si>
   <si>
+    <t>rushikesh.kurundwade24@pccoepune.org</t>
+  </si>
+  <si>
     <t>Durvas Bhadane</t>
   </si>
   <si>
@@ -5536,9 +5557,15 @@
     <t>Kuldeep Gheghate</t>
   </si>
   <si>
+    <t>kuldeep.gheghate23@pccoepune.org</t>
+  </si>
+  <si>
     <t>Harsh Asalkar</t>
   </si>
   <si>
+    <t>harsh.asalkar23@pccoepune.org</t>
+  </si>
+  <si>
     <t>Pranav Shirode</t>
   </si>
   <si>
@@ -5551,6 +5578,9 @@
     <t>Nandini Patil</t>
   </si>
   <si>
+    <t>nandini.patil24@pccoepune.org</t>
+  </si>
+  <si>
     <t>prerna.shirsath@pccoepune.org</t>
   </si>
   <si>
@@ -5584,6 +5614,9 @@
     <t>Chaitanya.atale24@pccoepune.org</t>
   </si>
   <si>
+    <t>om.kadu24@pccoepune.org</t>
+  </si>
+  <si>
     <t>somesh.abande 24@pccoepune.org</t>
   </si>
   <si>
@@ -5632,9 +5665,6 @@
     <t>sohan.metil23@gmail.com</t>
   </si>
   <si>
-    <t>ashish.patil23@pccoepune.org</t>
-  </si>
-  <si>
     <t>Vedant Takalkar</t>
   </si>
   <si>
@@ -5668,9 +5698,6 @@
     <t>kekansakshi@gmail.com</t>
   </si>
   <si>
-    <t>kuldeep.gheghate23@pccoepune.org</t>
-  </si>
-  <si>
     <t>Pratik Sukale</t>
   </si>
   <si>
@@ -5701,9 +5728,6 @@
     <t>Disha Andre</t>
   </si>
   <si>
-    <t>prajwal.hage23@pccoepune.org</t>
-  </si>
-  <si>
     <t>Yash Said</t>
   </si>
   <si>
@@ -5726,9 +5750,6 @@
   </si>
   <si>
     <t>mayurkarad99@gmail.com</t>
-  </si>
-  <si>
-    <t>harsh.asalkar23@pccoepune.org</t>
   </si>
   <si>
     <t>Aditya Vedpathak</t>
@@ -6137,7 +6158,6 @@
     <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -6150,6 +6170,7 @@
     <xf borderId="7" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
+    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -6184,16 +6205,20 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="3">
+  <tableStyles count="4">
     <tableStyle count="2" pivot="0" name="Sheet1-style">
       <tableStyleElement dxfId="1" type="firstRowStripe"/>
       <tableStyleElement dxfId="2" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="2" pivot="0" name="Sheet1-style 2">
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Sheet1-style 3">
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="1" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle count="2" pivot="0" name="Sheet1-style 3">
+    <tableStyle count="2" pivot="0" name="Sheet1-style 4">
       <tableStyleElement dxfId="1" type="firstRowStripe"/>
       <tableStyleElement dxfId="2" type="secondRowStripe"/>
     </tableStyle>
@@ -6206,7 +6231,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="C2:C1282" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="C2:C1289" displayName="Table_1" name="Table_1" id="1">
   <tableColumns count="1">
     <tableColumn name="Column1" id="1"/>
   </tableColumns>
@@ -6215,7 +6240,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="C1297:C1312" displayName="Table_2" name="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="C1293:C1296" displayName="Table_2" name="Table_2" id="2">
   <tableColumns count="1">
     <tableColumn name="Column1" id="1"/>
   </tableColumns>
@@ -6224,11 +6249,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="C1317:C1442" displayName="Table_3" name="Table_3" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="C1297:C1313" displayName="Table_3" name="Table_3" id="3">
   <tableColumns count="1">
     <tableColumn name="Column1" id="1"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="C1317:C1442" displayName="Table_4" name="Table_4" id="4">
+  <tableColumns count="1">
+    <tableColumn name="Column1" id="1"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet1-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -20055,6 +20089,9 @@
       <c r="B1238" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1238" s="3" t="s">
+        <v>1655</v>
+      </c>
     </row>
     <row r="1239">
       <c r="A1239" s="2" t="s">
@@ -20063,7 +20100,9 @@
       <c r="B1239" s="2" t="s">
         <v>1808</v>
       </c>
-      <c r="C1239" s="10"/>
+      <c r="C1239" s="4" t="s">
+        <v>1272</v>
+      </c>
     </row>
     <row r="1240">
       <c r="A1240" s="2" t="s">
@@ -20072,6 +20111,9 @@
       <c r="B1240" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1240" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="1241">
       <c r="A1241" s="2" t="s">
@@ -20080,7 +20122,9 @@
       <c r="B1241" s="2" t="s">
         <v>1808</v>
       </c>
-      <c r="C1241" s="10"/>
+      <c r="C1241" s="4" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="1242">
       <c r="A1242" s="2" t="s">
@@ -20089,6 +20133,9 @@
       <c r="B1242" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1242" s="3" t="s">
+        <v>1812</v>
+      </c>
     </row>
     <row r="1243">
       <c r="A1243" s="2" t="s">
@@ -20097,6 +20144,9 @@
       <c r="B1243" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1243" s="4" t="s">
+        <v>1663</v>
+      </c>
     </row>
     <row r="1244">
       <c r="A1244" s="2" t="s">
@@ -20105,10 +20155,13 @@
       <c r="B1244" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1244" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="1245">
       <c r="A1245" s="2" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="B1245" s="2" t="s">
         <v>1808</v>
@@ -20124,6 +20177,9 @@
       <c r="B1246" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1246" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="1247">
       <c r="A1247" s="2" t="s">
@@ -20132,6 +20188,9 @@
       <c r="B1247" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1247" s="4" t="s">
+        <v>1814</v>
+      </c>
     </row>
     <row r="1248">
       <c r="A1248" s="2" t="s">
@@ -20141,7 +20200,7 @@
         <v>1808</v>
       </c>
       <c r="C1248" s="4" t="s">
-        <v>1813</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="1249">
@@ -20157,7 +20216,7 @@
     </row>
     <row r="1250">
       <c r="A1250" s="2" t="s">
-        <v>1814</v>
+        <v>1816</v>
       </c>
       <c r="B1250" s="2" t="s">
         <v>1808</v>
@@ -20173,16 +20232,19 @@
       <c r="B1251" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1251" s="2" t="s">
+        <v>1159</v>
+      </c>
     </row>
     <row r="1252">
       <c r="A1252" s="2" t="s">
-        <v>1815</v>
+        <v>1817</v>
       </c>
       <c r="B1252" s="2" t="s">
         <v>1808</v>
       </c>
       <c r="C1252" s="3" t="s">
-        <v>1816</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="1253">
@@ -20198,18 +20260,24 @@
     </row>
     <row r="1254">
       <c r="A1254" s="2" t="s">
-        <v>1817</v>
+        <v>1819</v>
       </c>
       <c r="B1254" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1254" s="3" t="s">
+        <v>1820</v>
+      </c>
     </row>
     <row r="1255">
       <c r="A1255" s="2" t="s">
-        <v>1818</v>
+        <v>1821</v>
       </c>
       <c r="B1255" s="2" t="s">
         <v>1808</v>
+      </c>
+      <c r="C1255" s="4" t="s">
+        <v>1822</v>
       </c>
     </row>
     <row r="1256">
@@ -20219,18 +20287,24 @@
       <c r="B1256" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1256" s="3" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="1257">
       <c r="A1257" s="2" t="s">
-        <v>1819</v>
+        <v>1823</v>
       </c>
       <c r="B1257" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1257" s="4" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="1258">
       <c r="A1258" s="2" t="s">
-        <v>1820</v>
+        <v>1824</v>
       </c>
       <c r="B1258" s="2" t="s">
         <v>1808</v>
@@ -20241,13 +20315,13 @@
     </row>
     <row r="1259">
       <c r="A1259" s="2" t="s">
-        <v>1821</v>
+        <v>1825</v>
       </c>
       <c r="B1259" s="2" t="s">
         <v>1808</v>
       </c>
       <c r="C1259" s="4" t="s">
-        <v>1822</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="1260">
@@ -20263,7 +20337,7 @@
     </row>
     <row r="1261">
       <c r="A1261" s="2" t="s">
-        <v>1823</v>
+        <v>1827</v>
       </c>
       <c r="B1261" s="2" t="s">
         <v>1808</v>
@@ -20279,6 +20353,9 @@
       <c r="B1262" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1262" s="2" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="1263">
       <c r="A1263" s="2" t="s">
@@ -20337,7 +20414,7 @@
     </row>
     <row r="1268">
       <c r="A1268" s="2" t="s">
-        <v>1824</v>
+        <v>1828</v>
       </c>
       <c r="B1268" s="2" t="s">
         <v>1808</v>
@@ -20348,7 +20425,7 @@
     </row>
     <row r="1269">
       <c r="A1269" s="2" t="s">
-        <v>1825</v>
+        <v>1829</v>
       </c>
       <c r="B1269" s="2" t="s">
         <v>1808</v>
@@ -20359,7 +20436,7 @@
     </row>
     <row r="1270">
       <c r="A1270" s="2" t="s">
-        <v>1826</v>
+        <v>1830</v>
       </c>
       <c r="B1270" s="2" t="s">
         <v>1808</v>
@@ -20370,7 +20447,7 @@
     </row>
     <row r="1271">
       <c r="A1271" s="2" t="s">
-        <v>1827</v>
+        <v>1831</v>
       </c>
       <c r="B1271" s="2" t="s">
         <v>1808</v>
@@ -20381,7 +20458,7 @@
     </row>
     <row r="1272">
       <c r="A1272" s="2" t="s">
-        <v>1828</v>
+        <v>1832</v>
       </c>
       <c r="B1272" s="2" t="s">
         <v>1808</v>
@@ -20403,37 +20480,40 @@
     </row>
     <row r="1274">
       <c r="A1274" s="2" t="s">
-        <v>1829</v>
+        <v>1833</v>
       </c>
       <c r="B1274" s="2" t="s">
         <v>1808</v>
       </c>
       <c r="C1274" s="4" t="s">
-        <v>1830</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="1275">
       <c r="A1275" s="2" t="s">
-        <v>1831</v>
+        <v>1835</v>
       </c>
       <c r="B1275" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1275" s="2" t="s">
+        <v>1836</v>
+      </c>
     </row>
     <row r="1276">
       <c r="A1276" s="2" t="s">
-        <v>1832</v>
+        <v>1837</v>
       </c>
       <c r="B1276" s="2" t="s">
         <v>1808</v>
       </c>
       <c r="C1276" s="3" t="s">
-        <v>1833</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="1277">
       <c r="A1277" s="2" t="s">
-        <v>1834</v>
+        <v>1839</v>
       </c>
       <c r="B1277" s="2" t="s">
         <v>1808</v>
@@ -20455,7 +20535,7 @@
     </row>
     <row r="1279">
       <c r="A1279" s="2" t="s">
-        <v>1835</v>
+        <v>1840</v>
       </c>
       <c r="B1279" s="2" t="s">
         <v>1808</v>
@@ -20466,10 +20546,13 @@
     </row>
     <row r="1280">
       <c r="A1280" s="2" t="s">
-        <v>1836</v>
+        <v>1841</v>
       </c>
       <c r="B1280" s="2" t="s">
         <v>1808</v>
+      </c>
+      <c r="C1280" s="2" t="s">
+        <v>1842</v>
       </c>
     </row>
     <row r="1281">
@@ -20501,6 +20584,9 @@
       <c r="B1283" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1283" s="3" t="s">
+        <v>1704</v>
+      </c>
     </row>
     <row r="1284">
       <c r="A1284" s="2" t="s">
@@ -20509,13 +20595,19 @@
       <c r="B1284" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1284" s="4" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="1285">
       <c r="A1285" s="2" t="s">
-        <v>1837</v>
+        <v>1843</v>
       </c>
       <c r="B1285" s="2" t="s">
         <v>1808</v>
+      </c>
+      <c r="C1285" s="3" t="s">
+        <v>1844</v>
       </c>
     </row>
     <row r="1286">
@@ -20525,6 +20617,9 @@
       <c r="B1286" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1286" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="1287">
       <c r="A1287" s="2" t="s">
@@ -20533,6 +20628,9 @@
       <c r="B1287" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1287" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="1288">
       <c r="A1288" s="2" t="s">
@@ -20541,13 +20639,19 @@
       <c r="B1288" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1288" s="3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="1289">
       <c r="A1289" s="2" t="s">
-        <v>1838</v>
+        <v>1845</v>
       </c>
       <c r="B1289" s="2" t="s">
         <v>1808</v>
+      </c>
+      <c r="C1289" s="4" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="1290">
@@ -20568,10 +20672,13 @@
       <c r="B1291" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1291" s="2" t="s">
+        <v>883</v>
+      </c>
     </row>
     <row r="1292">
       <c r="A1292" s="2" t="s">
-        <v>1839</v>
+        <v>1846</v>
       </c>
       <c r="B1292" s="2" t="s">
         <v>1808</v>
@@ -20582,18 +20689,24 @@
     </row>
     <row r="1293">
       <c r="A1293" s="2" t="s">
-        <v>1840</v>
+        <v>1847</v>
       </c>
       <c r="B1293" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1293" s="3" t="s">
+        <v>1848</v>
+      </c>
     </row>
     <row r="1294">
       <c r="A1294" s="2" t="s">
-        <v>1841</v>
+        <v>1849</v>
       </c>
       <c r="B1294" s="2" t="s">
         <v>1808</v>
+      </c>
+      <c r="C1294" s="4" t="s">
+        <v>1850</v>
       </c>
     </row>
     <row r="1295">
@@ -20603,24 +20716,30 @@
       <c r="B1295" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1295" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="1296">
       <c r="A1296" s="2" t="s">
-        <v>1842</v>
+        <v>1851</v>
       </c>
       <c r="B1296" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1296" s="4" t="s">
+        <v>1408</v>
+      </c>
     </row>
     <row r="1297">
       <c r="A1297" s="2" t="s">
-        <v>1843</v>
+        <v>1852</v>
       </c>
       <c r="B1297" s="2" t="s">
         <v>1808</v>
       </c>
       <c r="C1297" s="4" t="s">
-        <v>1844</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="1298">
@@ -20647,10 +20766,13 @@
     </row>
     <row r="1300">
       <c r="A1300" s="2" t="s">
-        <v>1845</v>
+        <v>1854</v>
       </c>
       <c r="B1300" s="2" t="s">
         <v>1808</v>
+      </c>
+      <c r="C1300" s="2" t="s">
+        <v>1855</v>
       </c>
     </row>
     <row r="1301">
@@ -20694,7 +20816,7 @@
         <v>1808</v>
       </c>
       <c r="C1304" s="3" t="s">
-        <v>1846</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="1305">
@@ -20710,7 +20832,7 @@
     </row>
     <row r="1306">
       <c r="A1306" s="2" t="s">
-        <v>1847</v>
+        <v>1857</v>
       </c>
       <c r="B1306" s="2" t="s">
         <v>1808</v>
@@ -20721,29 +20843,29 @@
     </row>
     <row r="1307">
       <c r="A1307" s="2" t="s">
-        <v>1848</v>
+        <v>1858</v>
       </c>
       <c r="B1307" s="2" t="s">
         <v>1808</v>
       </c>
       <c r="C1307" s="4" t="s">
-        <v>1849</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="1308">
       <c r="A1308" s="2" t="s">
-        <v>1850</v>
+        <v>1860</v>
       </c>
       <c r="B1308" s="2" t="s">
         <v>1808</v>
       </c>
       <c r="C1308" s="3" t="s">
-        <v>1851</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="1309">
       <c r="A1309" s="2" t="s">
-        <v>1852</v>
+        <v>1862</v>
       </c>
       <c r="B1309" s="2" t="s">
         <v>1808</v>
@@ -20754,13 +20876,13 @@
     </row>
     <row r="1310">
       <c r="A1310" s="2" t="s">
-        <v>1853</v>
+        <v>1863</v>
       </c>
       <c r="B1310" s="2" t="s">
         <v>1808</v>
       </c>
       <c r="C1310" s="2" t="s">
-        <v>1854</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="1311">
@@ -20776,13 +20898,13 @@
     </row>
     <row r="1312">
       <c r="A1312" s="2" t="s">
-        <v>1855</v>
+        <v>1865</v>
       </c>
       <c r="B1312" s="2" t="s">
         <v>1808</v>
       </c>
       <c r="C1312" s="4" t="s">
-        <v>1856</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="1313">
@@ -20792,6 +20914,9 @@
       <c r="B1313" s="2" t="s">
         <v>1808</v>
       </c>
+      <c r="C1313" s="2" t="s">
+        <v>1867</v>
+      </c>
     </row>
     <row r="1314">
       <c r="A1314" s="2" t="s">
@@ -20801,20 +20926,20 @@
         <v>1808</v>
       </c>
       <c r="C1314" s="2" t="s">
-        <v>1857</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="1315">
-      <c r="A1315" s="11" t="s">
-        <v>1858</v>
+      <c r="A1315" s="10" t="s">
+        <v>1869</v>
       </c>
       <c r="B1315" s="2" t="s">
         <v>1808</v>
       </c>
     </row>
     <row r="1316">
-      <c r="A1316" s="11" t="s">
-        <v>1859</v>
+      <c r="A1316" s="10" t="s">
+        <v>1870</v>
       </c>
       <c r="B1316" s="2" t="s">
         <v>1808</v>
@@ -20822,10 +20947,10 @@
     </row>
     <row r="1317">
       <c r="A1317" s="2" t="s">
-        <v>1860</v>
+        <v>1871</v>
       </c>
       <c r="B1317" s="2" t="s">
-        <v>1861</v>
+        <v>1872</v>
       </c>
       <c r="C1317" s="3" t="s">
         <v>1658</v>
@@ -20833,13 +20958,13 @@
     </row>
     <row r="1318">
       <c r="A1318" s="2" t="s">
-        <v>1862</v>
+        <v>1873</v>
       </c>
       <c r="B1318" s="2" t="s">
-        <v>1861</v>
+        <v>1872</v>
       </c>
       <c r="C1318" s="4" t="s">
-        <v>1863</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="1319">
@@ -20847,7 +20972,7 @@
         <v>476</v>
       </c>
       <c r="B1319" s="2" t="s">
-        <v>1861</v>
+        <v>1872</v>
       </c>
       <c r="C1319" s="3" t="s">
         <v>477</v>
@@ -20855,13 +20980,13 @@
     </row>
     <row r="1320">
       <c r="A1320" s="2" t="s">
-        <v>1864</v>
+        <v>1875</v>
       </c>
       <c r="B1320" s="2" t="s">
-        <v>1861</v>
+        <v>1872</v>
       </c>
       <c r="C1320" s="4" t="s">
-        <v>1865</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="1321">
@@ -20869,7 +20994,7 @@
         <v>1542</v>
       </c>
       <c r="B1321" s="2" t="s">
-        <v>1861</v>
+        <v>1872</v>
       </c>
       <c r="C1321" s="3" t="s">
         <v>1218</v>
@@ -20880,9 +21005,9 @@
         <v>641</v>
       </c>
       <c r="B1322" s="2" t="s">
-        <v>1861</v>
-      </c>
-      <c r="C1322" s="11" t="s">
+        <v>1872</v>
+      </c>
+      <c r="C1322" s="10" t="s">
         <v>642</v>
       </c>
     </row>
@@ -20891,9 +21016,9 @@
         <v>1706</v>
       </c>
       <c r="B1323" s="2" t="s">
-        <v>1861</v>
-      </c>
-      <c r="C1323" s="11" t="s">
+        <v>1872</v>
+      </c>
+      <c r="C1323" s="10" t="s">
         <v>1707</v>
       </c>
     </row>
@@ -20902,7 +21027,7 @@
         <v>1659</v>
       </c>
       <c r="B1324" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1324" s="3" t="s">
         <v>1660</v>
@@ -20910,13 +21035,13 @@
     </row>
     <row r="1325">
       <c r="A1325" s="2" t="s">
-        <v>1867</v>
+        <v>1878</v>
       </c>
       <c r="B1325" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1325" s="4" t="s">
-        <v>1868</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="1326">
@@ -20924,7 +21049,7 @@
         <v>8</v>
       </c>
       <c r="B1326" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1326" s="3" t="s">
         <v>9</v>
@@ -20932,79 +21057,79 @@
     </row>
     <row r="1327">
       <c r="A1327" s="2" t="s">
-        <v>1869</v>
+        <v>1880</v>
       </c>
       <c r="B1327" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1327" s="4" t="s">
-        <v>1870</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="1328">
       <c r="A1328" s="2" t="s">
-        <v>1871</v>
+        <v>1882</v>
       </c>
       <c r="B1328" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1328" s="3" t="s">
-        <v>1872</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="1329">
       <c r="A1329" s="2" t="s">
-        <v>1817</v>
+        <v>1819</v>
       </c>
       <c r="B1329" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1329" s="4" t="s">
-        <v>1873</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="1330">
       <c r="A1330" s="2" t="s">
-        <v>1874</v>
+        <v>1884</v>
       </c>
       <c r="B1330" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1330" s="3" t="s">
-        <v>1875</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="1331">
       <c r="A1331" s="2" t="s">
-        <v>1826</v>
+        <v>1830</v>
       </c>
       <c r="B1331" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1331" s="4" t="s">
-        <v>1876</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="1332">
       <c r="A1332" s="2" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B1332" s="2" t="s">
         <v>1877</v>
       </c>
-      <c r="B1332" s="2" t="s">
-        <v>1866</v>
-      </c>
       <c r="C1332" s="3" t="s">
-        <v>1878</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="1333">
       <c r="A1333" s="2" t="s">
-        <v>1879</v>
+        <v>1889</v>
       </c>
       <c r="B1333" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1333" s="4" t="s">
-        <v>1880</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="1334">
@@ -21012,7 +21137,7 @@
         <v>1468</v>
       </c>
       <c r="B1334" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1334" s="3" t="s">
         <v>1469</v>
@@ -21020,10 +21145,10 @@
     </row>
     <row r="1335">
       <c r="A1335" s="2" t="s">
-        <v>1881</v>
+        <v>1891</v>
       </c>
       <c r="B1335" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1335" s="4" t="s">
         <v>955</v>
@@ -21034,7 +21159,7 @@
         <v>1093</v>
       </c>
       <c r="B1336" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1336" s="9" t="s">
         <v>1094</v>
@@ -21045,7 +21170,7 @@
         <v>1708</v>
       </c>
       <c r="B1337" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1337" s="3" t="s">
         <v>324</v>
@@ -21053,10 +21178,10 @@
     </row>
     <row r="1338">
       <c r="A1338" s="2" t="s">
-        <v>1882</v>
+        <v>1892</v>
       </c>
       <c r="B1338" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1338" s="3" t="s">
         <v>336</v>
@@ -21064,13 +21189,13 @@
     </row>
     <row r="1339">
       <c r="A1339" s="2" t="s">
-        <v>1883</v>
+        <v>1893</v>
       </c>
       <c r="B1339" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1339" s="4" t="s">
-        <v>1884</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="1340">
@@ -21078,7 +21203,7 @@
         <v>882</v>
       </c>
       <c r="B1340" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1340" s="3" t="s">
         <v>883</v>
@@ -21086,32 +21211,32 @@
     </row>
     <row r="1341">
       <c r="A1341" s="2" t="s">
-        <v>1840</v>
+        <v>1847</v>
       </c>
       <c r="B1341" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1341" s="4" t="s">
-        <v>1885</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="1342">
       <c r="A1342" s="2" t="s">
-        <v>1886</v>
+        <v>1895</v>
       </c>
       <c r="B1342" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1342" s="3" t="s">
-        <v>1887</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="1343">
       <c r="A1343" s="2" t="s">
-        <v>1888</v>
+        <v>1897</v>
       </c>
       <c r="B1343" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1343" s="4" t="s">
         <v>1275</v>
@@ -21119,24 +21244,24 @@
     </row>
     <row r="1344">
       <c r="A1344" s="2" t="s">
-        <v>1889</v>
+        <v>1898</v>
       </c>
       <c r="B1344" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1344" s="3" t="s">
-        <v>1890</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="1345">
       <c r="A1345" s="2" t="s">
-        <v>1891</v>
+        <v>1900</v>
       </c>
       <c r="B1345" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1345" s="4" t="s">
-        <v>1892</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="1346">
@@ -21144,7 +21269,7 @@
         <v>1479</v>
       </c>
       <c r="B1346" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1346" s="3" t="s">
         <v>1480</v>
@@ -21155,7 +21280,7 @@
         <v>812</v>
       </c>
       <c r="B1347" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1347" s="9" t="s">
         <v>813</v>
@@ -21163,21 +21288,21 @@
     </row>
     <row r="1348">
       <c r="A1348" s="2" t="s">
-        <v>1893</v>
+        <v>1902</v>
       </c>
       <c r="B1348" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1348" s="2" t="s">
-        <v>1894</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="1349">
       <c r="A1349" s="2" t="s">
-        <v>1895</v>
+        <v>1904</v>
       </c>
       <c r="B1349" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1349" s="2" t="s">
         <v>795</v>
@@ -21185,46 +21310,46 @@
     </row>
     <row r="1350">
       <c r="A1350" s="2" t="s">
-        <v>1818</v>
+        <v>1821</v>
       </c>
       <c r="B1350" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1350" s="2" t="s">
-        <v>1896</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="1351">
       <c r="A1351" s="2" t="s">
-        <v>1897</v>
+        <v>1905</v>
       </c>
       <c r="B1351" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1351" s="2" t="s">
-        <v>1898</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="1352">
       <c r="A1352" s="2" t="s">
-        <v>1899</v>
+        <v>1907</v>
       </c>
       <c r="B1352" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1352" s="2" t="s">
-        <v>1900</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="1353">
       <c r="A1353" s="2" t="s">
-        <v>1901</v>
+        <v>1909</v>
       </c>
       <c r="B1353" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1353" s="2" t="s">
-        <v>1902</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="1354">
@@ -21232,7 +21357,7 @@
         <v>1368</v>
       </c>
       <c r="B1354" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1354" s="2" t="s">
         <v>1034</v>
@@ -21240,46 +21365,46 @@
     </row>
     <row r="1355">
       <c r="A1355" s="2" t="s">
-        <v>1903</v>
+        <v>1911</v>
       </c>
       <c r="B1355" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1355" s="2" t="s">
-        <v>1904</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="1356">
       <c r="A1356" s="2" t="s">
-        <v>1841</v>
+        <v>1849</v>
       </c>
       <c r="B1356" s="2" t="s">
-        <v>1866</v>
-      </c>
-      <c r="C1356" s="12" t="s">
-        <v>1905</v>
+        <v>1877</v>
+      </c>
+      <c r="C1356" s="11" t="s">
+        <v>1850</v>
       </c>
     </row>
     <row r="1357">
       <c r="A1357" s="2" t="s">
-        <v>1906</v>
+        <v>1913</v>
       </c>
       <c r="B1357" s="2" t="s">
-        <v>1866</v>
-      </c>
-      <c r="C1357" s="13" t="s">
-        <v>1907</v>
+        <v>1877</v>
+      </c>
+      <c r="C1357" s="12" t="s">
+        <v>1914</v>
       </c>
     </row>
     <row r="1358">
       <c r="A1358" s="2" t="s">
-        <v>1908</v>
+        <v>1915</v>
       </c>
       <c r="B1358" s="2" t="s">
-        <v>1866</v>
+        <v>1877</v>
       </c>
       <c r="C1358" s="2" t="s">
-        <v>1909</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="1359">
@@ -21287,7 +21412,7 @@
         <v>1703</v>
       </c>
       <c r="B1359" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1359" s="3" t="s">
         <v>1704</v>
@@ -21298,7 +21423,7 @@
         <v>14</v>
       </c>
       <c r="B1360" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1360" s="4" t="s">
         <v>15</v>
@@ -21309,7 +21434,7 @@
         <v>655</v>
       </c>
       <c r="B1361" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1361" s="3" t="s">
         <v>656</v>
@@ -21320,7 +21445,7 @@
         <v>667</v>
       </c>
       <c r="B1362" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1362" s="4" t="s">
         <v>668</v>
@@ -21331,7 +21456,7 @@
         <v>689</v>
       </c>
       <c r="B1363" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1363" s="3" t="s">
         <v>690</v>
@@ -21339,10 +21464,10 @@
     </row>
     <row r="1364">
       <c r="A1364" s="2" t="s">
-        <v>1911</v>
+        <v>1918</v>
       </c>
       <c r="B1364" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1364" s="4" t="s">
         <v>1212</v>
@@ -21353,7 +21478,7 @@
         <v>722</v>
       </c>
       <c r="B1365" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1365" s="3" t="s">
         <v>723</v>
@@ -21364,7 +21489,7 @@
         <v>724</v>
       </c>
       <c r="B1366" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1366" s="4" t="s">
         <v>725</v>
@@ -21375,7 +21500,7 @@
         <v>1557</v>
       </c>
       <c r="B1367" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1367" s="3" t="s">
         <v>416</v>
@@ -21383,13 +21508,13 @@
     </row>
     <row r="1368">
       <c r="A1368" s="2" t="s">
-        <v>1912</v>
+        <v>1919</v>
       </c>
       <c r="B1368" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1368" s="4" t="s">
-        <v>1913</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="1369">
@@ -21397,7 +21522,7 @@
         <v>753</v>
       </c>
       <c r="B1369" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1369" s="3" t="s">
         <v>754</v>
@@ -21408,7 +21533,7 @@
         <v>1195</v>
       </c>
       <c r="B1370" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1370" s="4" t="s">
         <v>1196</v>
@@ -21419,10 +21544,10 @@
         <v>1142</v>
       </c>
       <c r="B1371" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1371" s="3" t="s">
-        <v>1914</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="1372">
@@ -21430,7 +21555,7 @@
         <v>841</v>
       </c>
       <c r="B1372" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1372" s="4" t="s">
         <v>842</v>
@@ -21441,7 +21566,7 @@
         <v>712</v>
       </c>
       <c r="B1373" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1373" s="3" t="s">
         <v>713</v>
@@ -21452,7 +21577,7 @@
         <v>1213</v>
       </c>
       <c r="B1374" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1374" s="4" t="s">
         <v>1214</v>
@@ -21460,13 +21585,13 @@
     </row>
     <row r="1375">
       <c r="A1375" s="2" t="s">
-        <v>1915</v>
+        <v>1922</v>
       </c>
       <c r="B1375" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1375" s="3" t="s">
-        <v>1916</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="1376">
@@ -21474,7 +21599,7 @@
         <v>812</v>
       </c>
       <c r="B1376" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1376" s="4" t="s">
         <v>813</v>
@@ -21485,7 +21610,7 @@
         <v>1307</v>
       </c>
       <c r="B1377" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1377" s="3" t="s">
         <v>1308</v>
@@ -21493,10 +21618,10 @@
     </row>
     <row r="1378">
       <c r="A1378" s="2" t="s">
-        <v>1824</v>
+        <v>1828</v>
       </c>
       <c r="B1378" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1378" s="4" t="s">
         <v>830</v>
@@ -21507,7 +21632,7 @@
         <v>759</v>
       </c>
       <c r="B1379" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1379" s="3" t="s">
         <v>760</v>
@@ -21515,10 +21640,10 @@
     </row>
     <row r="1380">
       <c r="A1380" s="2" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B1380" s="2" t="s">
         <v>1917</v>
-      </c>
-      <c r="B1380" s="2" t="s">
-        <v>1910</v>
       </c>
       <c r="C1380" s="4" t="s">
         <v>1011</v>
@@ -21529,7 +21654,7 @@
         <v>1689</v>
       </c>
       <c r="B1381" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1381" s="3" t="s">
         <v>1209</v>
@@ -21540,7 +21665,7 @@
         <v>1313</v>
       </c>
       <c r="B1382" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1382" s="4" t="s">
         <v>1314</v>
@@ -21551,7 +21676,7 @@
         <v>859</v>
       </c>
       <c r="B1383" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1383" s="3" t="s">
         <v>860</v>
@@ -21559,32 +21684,32 @@
     </row>
     <row r="1384">
       <c r="A1384" s="2" t="s">
-        <v>1918</v>
+        <v>1925</v>
       </c>
       <c r="B1384" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1384" s="4" t="s">
-        <v>1919</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="1385">
       <c r="A1385" s="2" t="s">
-        <v>1850</v>
+        <v>1860</v>
       </c>
       <c r="B1385" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1385" s="3" t="s">
-        <v>1851</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="1386">
       <c r="A1386" s="2" t="s">
-        <v>1920</v>
+        <v>1927</v>
       </c>
       <c r="B1386" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1386" s="4" t="s">
         <v>1152</v>
@@ -21595,10 +21720,10 @@
         <v>403</v>
       </c>
       <c r="B1387" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1387" s="3" t="s">
-        <v>1921</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="1388">
@@ -21606,7 +21731,7 @@
         <v>1761</v>
       </c>
       <c r="B1388" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1388" s="4" t="s">
         <v>1762</v>
@@ -21614,13 +21739,13 @@
     </row>
     <row r="1389">
       <c r="A1389" s="2" t="s">
-        <v>1922</v>
+        <v>1929</v>
       </c>
       <c r="B1389" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1389" s="3" t="s">
-        <v>1923</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="1390">
@@ -21628,7 +21753,7 @@
         <v>16</v>
       </c>
       <c r="B1390" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1390" s="4" t="s">
         <v>17</v>
@@ -21639,7 +21764,7 @@
         <v>276</v>
       </c>
       <c r="B1391" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1391" s="3" t="s">
         <v>113</v>
@@ -21647,13 +21772,13 @@
     </row>
     <row r="1392">
       <c r="A1392" s="2" t="s">
-        <v>1924</v>
+        <v>1931</v>
       </c>
       <c r="B1392" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1392" s="4" t="s">
-        <v>1925</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="1393">
@@ -21661,10 +21786,10 @@
         <v>906</v>
       </c>
       <c r="B1393" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1393" s="3" t="s">
-        <v>1926</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="1394">
@@ -21672,7 +21797,7 @@
         <v>805</v>
       </c>
       <c r="B1394" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1394" s="4" t="s">
         <v>806</v>
@@ -21683,7 +21808,7 @@
         <v>1029</v>
       </c>
       <c r="B1395" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1395" s="3" t="s">
         <v>1030</v>
@@ -21694,7 +21819,7 @@
         <v>166</v>
       </c>
       <c r="B1396" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1396" s="7" t="s">
         <v>167</v>
@@ -21705,7 +21830,7 @@
         <v>1654</v>
       </c>
       <c r="B1397" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1397" s="3" t="s">
         <v>1655</v>
@@ -21716,7 +21841,7 @@
         <v>502</v>
       </c>
       <c r="B1398" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1398" s="4" t="s">
         <v>1770</v>
@@ -21724,13 +21849,13 @@
     </row>
     <row r="1399">
       <c r="A1399" s="2" t="s">
-        <v>1927</v>
+        <v>1934</v>
       </c>
       <c r="B1399" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1399" s="3" t="s">
-        <v>1928</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="1400">
@@ -21738,7 +21863,7 @@
         <v>942</v>
       </c>
       <c r="B1400" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1400" s="4" t="s">
         <v>943</v>
@@ -21749,7 +21874,7 @@
         <v>1236</v>
       </c>
       <c r="B1401" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1401" s="3" t="s">
         <v>1237</v>
@@ -21757,13 +21882,13 @@
     </row>
     <row r="1402">
       <c r="A1402" s="2" t="s">
-        <v>1929</v>
+        <v>1936</v>
       </c>
       <c r="B1402" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1402" s="4" t="s">
-        <v>1930</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="1403">
@@ -21771,7 +21896,7 @@
         <v>1003</v>
       </c>
       <c r="B1403" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1403" s="3" t="s">
         <v>1004</v>
@@ -21782,7 +21907,7 @@
         <v>1276</v>
       </c>
       <c r="B1404" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1404" s="4" t="s">
         <v>1277</v>
@@ -21790,10 +21915,10 @@
     </row>
     <row r="1405">
       <c r="A1405" s="2" t="s">
-        <v>1931</v>
+        <v>1938</v>
       </c>
       <c r="B1405" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1405" s="3" t="s">
         <v>91</v>
@@ -21804,7 +21929,7 @@
         <v>1465</v>
       </c>
       <c r="B1406" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1406" s="3" t="s">
         <v>1467</v>
@@ -21812,24 +21937,24 @@
     </row>
     <row r="1407">
       <c r="A1407" s="2" t="s">
-        <v>1932</v>
+        <v>1939</v>
       </c>
       <c r="B1407" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1407" s="4" t="s">
-        <v>1933</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="1408">
       <c r="A1408" s="2" t="s">
-        <v>1934</v>
+        <v>1941</v>
       </c>
       <c r="B1408" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1408" s="3" t="s">
-        <v>1935</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="1409">
@@ -21837,7 +21962,7 @@
         <v>1122</v>
       </c>
       <c r="B1409" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1409" s="4" t="s">
         <v>1123</v>
@@ -21845,10 +21970,10 @@
     </row>
     <row r="1410">
       <c r="A1410" s="2" t="s">
-        <v>1936</v>
+        <v>1943</v>
       </c>
       <c r="B1410" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1410" s="3" t="s">
         <v>992</v>
@@ -21856,10 +21981,10 @@
     </row>
     <row r="1411">
       <c r="A1411" s="2" t="s">
-        <v>1937</v>
+        <v>1944</v>
       </c>
       <c r="B1411" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1411" s="4" t="s">
         <v>1677</v>
@@ -21870,7 +21995,7 @@
         <v>1093</v>
       </c>
       <c r="B1412" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1412" s="4" t="s">
         <v>1094</v>
@@ -21881,10 +22006,10 @@
         <v>1477</v>
       </c>
       <c r="B1413" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1413" s="3" t="s">
-        <v>1938</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="1414">
@@ -21892,7 +22017,7 @@
         <v>1381</v>
       </c>
       <c r="B1414" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1414" s="4" t="s">
         <v>1470</v>
@@ -21903,7 +22028,7 @@
         <v>1261</v>
       </c>
       <c r="B1415" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1415" s="3" t="s">
         <v>1262</v>
@@ -21914,7 +22039,7 @@
         <v>1705</v>
       </c>
       <c r="B1416" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1416" s="3" t="s">
         <v>664</v>
@@ -21925,7 +22050,7 @@
         <v>845</v>
       </c>
       <c r="B1417" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1417" s="4" t="s">
         <v>846</v>
@@ -21936,7 +22061,7 @@
         <v>1139</v>
       </c>
       <c r="B1418" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1418" s="3" t="s">
         <v>1140</v>
@@ -21944,13 +22069,13 @@
     </row>
     <row r="1419">
       <c r="A1419" s="2" t="s">
-        <v>1939</v>
+        <v>1946</v>
       </c>
       <c r="B1419" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1419" s="8" t="s">
-        <v>1940</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="1420">
@@ -21958,7 +22083,7 @@
         <v>1164</v>
       </c>
       <c r="B1420" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1420" s="3" t="s">
         <v>1165</v>
@@ -21966,10 +22091,10 @@
     </row>
     <row r="1421">
       <c r="A1421" s="2" t="s">
-        <v>1941</v>
+        <v>1948</v>
       </c>
       <c r="B1421" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1421" s="4" t="s">
         <v>873</v>
@@ -21977,13 +22102,13 @@
     </row>
     <row r="1422">
       <c r="A1422" s="2" t="s">
-        <v>1942</v>
+        <v>1949</v>
       </c>
       <c r="B1422" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1422" s="3" t="s">
-        <v>1943</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="1423">
@@ -21991,7 +22116,7 @@
         <v>1298</v>
       </c>
       <c r="B1423" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1423" s="4" t="s">
         <v>1299</v>
@@ -21999,13 +22124,13 @@
     </row>
     <row r="1424">
       <c r="A1424" s="2" t="s">
-        <v>1944</v>
+        <v>1951</v>
       </c>
       <c r="B1424" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1424" s="3" t="s">
-        <v>1945</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="1425">
@@ -22013,7 +22138,7 @@
         <v>180</v>
       </c>
       <c r="B1425" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1425" s="4" t="s">
         <v>181</v>
@@ -22021,10 +22146,10 @@
     </row>
     <row r="1426">
       <c r="A1426" s="2" t="s">
-        <v>1946</v>
+        <v>1953</v>
       </c>
       <c r="B1426" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1426" s="3" t="s">
         <v>113</v>
@@ -22032,21 +22157,21 @@
     </row>
     <row r="1427">
       <c r="A1427" s="2" t="s">
-        <v>1947</v>
+        <v>1954</v>
       </c>
       <c r="B1427" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1427" s="4" t="s">
-        <v>1948</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="1428">
       <c r="A1428" s="2" t="s">
-        <v>1949</v>
+        <v>1956</v>
       </c>
       <c r="B1428" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1428" s="3" t="s">
         <v>1183</v>
@@ -22057,10 +22182,10 @@
         <v>1337</v>
       </c>
       <c r="B1429" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1429" s="4" t="s">
-        <v>1950</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="1430">
@@ -22068,7 +22193,7 @@
         <v>745</v>
       </c>
       <c r="B1430" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1430" s="3" t="s">
         <v>746</v>
@@ -22076,21 +22201,21 @@
     </row>
     <row r="1431">
       <c r="A1431" s="2" t="s">
-        <v>1951</v>
+        <v>1958</v>
       </c>
       <c r="B1431" s="2" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="C1431" s="7" t="s">
-        <v>1952</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="1432">
       <c r="A1432" s="2" t="s">
-        <v>1953</v>
+        <v>1960</v>
       </c>
       <c r="B1432" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
       <c r="C1432" s="3" t="s">
         <v>811</v>
@@ -22101,40 +22226,40 @@
         <v>814</v>
       </c>
       <c r="B1433" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
       <c r="C1433" s="4" t="s">
-        <v>1955</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="1434">
       <c r="A1434" s="2" t="s">
-        <v>1956</v>
+        <v>1963</v>
       </c>
       <c r="B1434" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
       <c r="C1434" s="3" t="s">
-        <v>1957</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="1435">
       <c r="A1435" s="2" t="s">
-        <v>1958</v>
+        <v>1965</v>
       </c>
       <c r="B1435" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
       <c r="C1435" s="4" t="s">
-        <v>1959</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="1436">
       <c r="A1436" s="2" t="s">
-        <v>1960</v>
+        <v>1967</v>
       </c>
       <c r="B1436" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
       <c r="C1436" s="3" t="s">
         <v>47</v>
@@ -22142,24 +22267,24 @@
     </row>
     <row r="1437">
       <c r="A1437" s="2" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B1437" s="2" t="s">
         <v>1961</v>
       </c>
-      <c r="B1437" s="2" t="s">
-        <v>1954</v>
-      </c>
       <c r="C1437" s="4" t="s">
-        <v>1962</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="1438">
       <c r="A1438" s="2" t="s">
-        <v>1963</v>
+        <v>1970</v>
       </c>
       <c r="B1438" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
       <c r="C1438" s="3" t="s">
-        <v>1964</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="1439">
@@ -22167,7 +22292,7 @@
         <v>853</v>
       </c>
       <c r="B1439" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
       <c r="C1439" s="4" t="s">
         <v>854</v>
@@ -22175,87 +22300,87 @@
     </row>
     <row r="1440">
       <c r="A1440" s="2" t="s">
-        <v>1965</v>
+        <v>1972</v>
       </c>
       <c r="B1440" s="2" t="s">
-        <v>1954</v>
-      </c>
-      <c r="C1440" s="14" t="s">
-        <v>1966</v>
+        <v>1961</v>
+      </c>
+      <c r="C1440" s="13" t="s">
+        <v>1973</v>
       </c>
     </row>
     <row r="1441">
       <c r="A1441" s="2" t="s">
-        <v>1967</v>
+        <v>1974</v>
       </c>
       <c r="B1441" s="2" t="s">
-        <v>1954</v>
-      </c>
-      <c r="C1441" s="10"/>
+        <v>1961</v>
+      </c>
+      <c r="C1441" s="14"/>
     </row>
     <row r="1442">
       <c r="A1442" s="2" t="s">
-        <v>1968</v>
+        <v>1975</v>
       </c>
       <c r="B1442" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
       <c r="C1442" s="15"/>
     </row>
     <row r="1443">
       <c r="A1443" s="2" t="s">
-        <v>1969</v>
+        <v>1976</v>
       </c>
       <c r="B1443" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="1444">
       <c r="A1444" s="2" t="s">
-        <v>1970</v>
+        <v>1977</v>
       </c>
       <c r="B1444" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="1445">
       <c r="A1445" s="2" t="s">
-        <v>1971</v>
+        <v>1978</v>
       </c>
       <c r="B1445" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="1446">
       <c r="A1446" s="2" t="s">
-        <v>1972</v>
+        <v>1979</v>
       </c>
       <c r="B1446" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="1447">
       <c r="A1447" s="2" t="s">
-        <v>1973</v>
+        <v>1980</v>
       </c>
       <c r="B1447" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="1448">
       <c r="A1448" s="2" t="s">
-        <v>1974</v>
+        <v>1981</v>
       </c>
       <c r="B1448" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="1449">
       <c r="A1449" s="2" t="s">
-        <v>1975</v>
+        <v>1982</v>
       </c>
       <c r="B1449" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="1450">
@@ -22263,7 +22388,7 @@
         <v>210</v>
       </c>
       <c r="B1450" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="1451">
@@ -22271,7 +22396,7 @@
         <v>1369</v>
       </c>
       <c r="B1451" s="2" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="1452">
@@ -23883,10 +24008,11 @@
     <hyperlink r:id="rId6" ref="C1024"/>
   </hyperlinks>
   <drawing r:id="rId7"/>
-  <tableParts count="3">
-    <tablePart r:id="rId11"/>
+  <tableParts count="4">
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>